<commit_message>
report 157-160, water and heat iot
</commit_message>
<xml_diff>
--- a/prizmer/static/excel/water_digital_template_for_load.xlsx
+++ b/prizmer/static/excel/water_digital_template_for_load.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
   <si>
     <t xml:space="preserve">Населенный пункт</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t xml:space="preserve">Пульсар IoT ВС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ХВС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">←тип прибора ХВС или ГВС</t>
   </si>
 </sst>
 </file>
@@ -288,7 +294,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -355,6 +361,10 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -586,7 +596,7 @@
   <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1086,6 +1096,14 @@
       <c r="N12" s="14" t="s">
         <v>20</v>
       </c>
+      <c r="O12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>